<commit_message>
update all scripts and data after reset
</commit_message>
<xml_diff>
--- a/wq/ToetsresultatenPrio2013-2018Meetpuntniveau.xlsx
+++ b/wq/ToetsresultatenPrio2013-2018Meetpuntniveau.xlsx
@@ -94297,4 +94297,411 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Algemeen - Word" ma:contentTypeID="0x0101004F34529632943E4DBB820B36F0ABAA0606010086381A6D56669A4DB59F7772448721B1" ma:contentTypeVersion="5" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="8fe95572a7a7878b61abe4cdcaa95a61">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d59e9867-4acc-40d5-91da-91f4047d1695" xmlns:ns3="fbe582d4-4cd9-4e01-adc0-428c7d30a990" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b624776c1a3c75443e1a1b758f5efa1" ns2:_="" ns3:_="">
+    <xsd:import namespace="d59e9867-4acc-40d5-91da-91f4047d1695"/>
+    <xsd:import namespace="fbe582d4-4cd9-4e01-adc0-428c7d30a990"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:Classificatie" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxKeywordTaxHTField" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
+                <xsd:element ref="ns2:Aanmaakdatum" minOccurs="0"/>
+                <xsd:element ref="ns2:Aggregatieniveau" minOccurs="0"/>
+                <xsd:element ref="ns2:Document_x0020_type" minOccurs="0"/>
+                <xsd:element ref="ns2:Entiteit_x0020_type" minOccurs="0"/>
+                <xsd:element ref="ns2:Identificatiekenmerk" minOccurs="0"/>
+                <xsd:element ref="ns2:Omschrijving" minOccurs="0"/>
+                <xsd:element ref="ns3:_dlc_DocId" minOccurs="0"/>
+                <xsd:element ref="ns3:_dlc_DocIdUrl" minOccurs="0"/>
+                <xsd:element ref="ns3:_dlc_DocIdPersistId" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d59e9867-4acc-40d5-91da-91f4047d1695" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Classificatie" ma:index="8" nillable="true" ma:displayName="Classificatie" ma:default="Openbaar" ma:format="Dropdown" ma:internalName="Classificatie">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Openbaar"/>
+          <xsd:enumeration value="Intern"/>
+          <xsd:enumeration value="Vertrouwelijk"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxKeywordTaxHTField" ma:index="9" nillable="true" ma:taxonomy="true" ma:internalName="TaxKeywordTaxHTField" ma:taxonomyFieldName="TaxKeyword" ma:displayName="Ondernemingstrefwoorden" ma:fieldId="{23f27201-bee3-471e-b2e7-b64fd8b7ca38}" ma:taxonomyMulti="true" ma:sspId="7c1d69d6-3248-424b-85a1-c0d9ad05b603" ma:termSetId="00000000-0000-0000-0000-000000000000" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="true" ma:isKeyword="true">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="10" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{0EFC20CD-FFEE-448C-92FD-8750F0F079A9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="{4053d47c-e7ab-4fe7-9faa-326c425f2d86}">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAllLabel" ma:index="11" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{0EFC20CD-FFEE-448C-92FD-8750F0F079A9}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="{4053d47c-e7ab-4fe7-9faa-326c425f2d86}">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Aanmaakdatum" ma:index="13" nillable="true" ma:displayName="Datum Document" ma:format="DateOnly" ma:internalName="Aanmaakdatum">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Aggregatieniveau" ma:index="14" nillable="true" ma:displayName="Aggregatieniveau" ma:default="Archiefstuk" ma:format="Dropdown" ma:internalName="Aggregatieniveau">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Archiefstuk"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Document_x0020_type" ma:index="15" nillable="true" ma:displayName="Document type" ma:format="Dropdown" ma:internalName="Document_x0020_type">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="AANGIFTE"/>
+          <xsd:enumeration value="AANMANING"/>
+          <xsd:enumeration value="AANMELDING"/>
+          <xsd:enumeration value="AANVRAAG"/>
+          <xsd:enumeration value="ADVIES"/>
+          <xsd:enumeration value="AFMELDING"/>
+          <xsd:enumeration value="AFSPRAAK"/>
+          <xsd:enumeration value="AGENDA"/>
+          <xsd:enumeration value="BEGELEIDEND SCHRIJVEN"/>
+          <xsd:enumeration value="BEGROTING"/>
+          <xsd:enumeration value="BENOEMING"/>
+          <xsd:enumeration value="BEROEPSCHRIFT"/>
+          <xsd:enumeration value="BESCHIKKING"/>
+          <xsd:enumeration value="BESLUIT"/>
+          <xsd:enumeration value="BESLUITENLIJST"/>
+          <xsd:enumeration value="BESTEK"/>
+          <xsd:enumeration value="BESTELLING"/>
+          <xsd:enumeration value="BESTEMMINGSPLAN"/>
+          <xsd:enumeration value="BETAALAFSPRAAK"/>
+          <xsd:enumeration value="BETAALOPDRACHT"/>
+          <xsd:enumeration value="BETALINGSHERINNERING"/>
+          <xsd:enumeration value="BEVESTIGING"/>
+          <xsd:enumeration value="BEZWAARSCHRIFT"/>
+          <xsd:enumeration value="CHECKLIST"/>
+          <xsd:enumeration value="DECLARATIE"/>
+          <xsd:enumeration value="FACTUUR"/>
+          <xsd:enumeration value="FILM"/>
+          <xsd:enumeration value="FOTO"/>
+          <xsd:enumeration value="GARANTIEBEWIJS"/>
+          <xsd:enumeration value="GESPREKSVERSLAG"/>
+          <xsd:enumeration value="GRAFIEK"/>
+          <xsd:enumeration value="HERINNERING"/>
+          <xsd:enumeration value="IDENTIFICATIEBEWIJS"/>
+          <xsd:enumeration value="KAART"/>
+          <xsd:enumeration value="KLACHT"/>
+          <xsd:enumeration value="mededeling"/>
+          <xsd:enumeration value="MELDING"/>
+          <xsd:enumeration value="NORM"/>
+          <xsd:enumeration value="NOTA"/>
+          <xsd:enumeration value="NOTITIE"/>
+          <xsd:enumeration value="OFFERTE"/>
+          <xsd:enumeration value="ONTWERP"/>
+          <xsd:enumeration value="OPDRACHT"/>
+          <xsd:enumeration value="OVEREENKOMST"/>
+          <xsd:enumeration value="PAKKET VAN EISEN"/>
+          <xsd:enumeration value="PLAN VAN AANPAK"/>
+          <xsd:enumeration value="PROCESBESCHRIJVING"/>
+          <xsd:enumeration value="PROCES-VERBAAL"/>
+          <xsd:enumeration value="RAPPORT"/>
+          <xsd:enumeration value="SOLLICITATIEBRIEF"/>
+          <xsd:enumeration value="TEKENING"/>
+          <xsd:enumeration value="VERGADERVERSLAG"/>
+          <xsd:enumeration value="VERGUNNING"/>
+          <xsd:enumeration value="VERKLARING"/>
+          <xsd:enumeration value="VERORDENING"/>
+          <xsd:enumeration value="VERSLAG"/>
+          <xsd:enumeration value="VERSLAG VAN BEVINDINGEN"/>
+          <xsd:enumeration value="VERZOEK"/>
+          <xsd:enumeration value="VERZOEKSCHRIFT"/>
+          <xsd:enumeration value="VOORDRACHT"/>
+          <xsd:enumeration value="VOORSCHRIFT"/>
+          <xsd:enumeration value="VOORSTEL"/>
+          <xsd:enumeration value="WET"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Entiteit_x0020_type" ma:index="16" nillable="true" ma:displayName="Entiteit type" ma:default="Record" ma:format="Dropdown" ma:internalName="Entiteit_x0020_type">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Record"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Identificatiekenmerk" ma:index="17" nillable="true" ma:displayName="Identificatiekenmerk" ma:description="Uniek kenmerk, door systeem gegenereerd" ma:internalName="Identificatiekenmerk">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Omschrijving" ma:index="18" nillable="true" ma:displayName="Omschrijving" ma:internalName="Omschrijving">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fbe582d4-4cd9-4e01-adc0-428c7d30a990" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_dlc_DocId" ma:index="19" nillable="true" ma:displayName="Waarde van de document-id" ma:description="De waarde van de document-id die aan dit item is toegewezen." ma:internalName="_dlc_DocId" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_dlc_DocIdUrl" ma:index="20" nillable="true" ma:displayName="Document-id" ma:description="Permanente koppeling naar dit document." ma:hidden="true" ma:internalName="_dlc_DocIdUrl" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:URL">
+            <xsd:sequence>
+              <xsd:element name="Url" type="dms:ValidUrl" minOccurs="0" nillable="true"/>
+              <xsd:element name="Description" type="xsd:string" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="_dlc_DocIdPersistId" ma:index="21" nillable="true" ma:displayName="Id blijven behouden" ma:description="Id behouden tijdens toevoegen." ma:hidden="true" ma:internalName="_dlc_DocIdPersistId" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhoudstype"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="7c1d69d6-3248-424b-85a1-c0d9ad05b603" ContentTypeId="0x0101004F34529632943E4DBB820B36F0ABAA060601" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Classificatie xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Intern</Classificatie>
+    <Entiteit_x0020_type xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Record</Entiteit_x0020_type>
+    <Aggregatieniveau xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Archiefstuk</Aggregatieniveau>
+    <_dlc_DocId xmlns="fbe582d4-4cd9-4e01-adc0-428c7d30a990">PNHZET2ZRHHM-1647798991-155236</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="fbe582d4-4cd9-4e01-adc0-428c7d30a990">
+      <Url>https://waternet.sharepoint.com/sites/0182/_layouts/15/DocIdRedir.aspx?ID=PNHZET2ZRHHM-1647798991-155236</Url>
+      <Description>PNHZET2ZRHHM-1647798991-155236</Description>
+    </_dlc_DocIdUrl>
+    <Identificatiekenmerk xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Aanmaakdatum xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
+    <TaxCatchAll xmlns="d59e9867-4acc-40d5-91da-91f4047d1695"/>
+    <Document_x0020_type xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
+    <Omschrijving xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D842F8-91D0-4DD5-8933-CCE42A42B3A4}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E76B79DB-EDEE-4F74-902C-A1916988FCD8}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0331C54D-B196-493D-95DF-B5BB28E3AF21}"/>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71211BBB-AB09-4891-82D7-452BFFE87C9E}"/>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{729BEA21-6A2E-46E1-9A93-CD727780710A}"/>
 </file>
</xml_diff>